<commit_message>
transferred semantic notes to NFDI4PSO
</commit_message>
<xml_diff>
--- a/templates/4COM01_RNASeq/4COM01_RNASeq.xlsx
+++ b/templates/4COM01_RNASeq/4COM01_RNASeq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/MetadataTemplates/SWATE_templates/templates/4COM01_RNASeq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3C35EA-13C6-7243-A1F5-2BFAD888676C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901B3493-265B-A845-B930-FD19F2142909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25100" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM01_RNASeq" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="116">
   <si>
     <t>Source Name</t>
   </si>
@@ -126,9 +126,6 @@
     <t>ER target term</t>
   </si>
   <si>
-    <t>Additional information</t>
-  </si>
-  <si>
     <t>User instruction</t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t>Trimmomatic</t>
   </si>
   <si>
-    <t>GENEPIO_0002096: read adapter trimming software</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0002096</t>
-  </si>
-  <si>
     <t>Kallisto</t>
   </si>
   <si>
@@ -235,9 +226,6 @@
   </si>
   <si>
     <t>SWATE_annotation_table</t>
-  </si>
-  <si>
-    <t>SWATE templating version (July 26, 2021)</t>
   </si>
   <si>
     <t>content_examples</t>
@@ -382,6 +370,21 @@
   </si>
   <si>
     <t>The format of the processed data file of this sample.</t>
+  </si>
+  <si>
+    <t>SWATE templating version (August 18, 2021)</t>
+  </si>
+  <si>
+    <t>is_a term</t>
+  </si>
+  <si>
+    <t>Use to specify subclasses of existing terms</t>
+  </si>
+  <si>
+    <t>is_a URI</t>
+  </si>
+  <si>
+    <t>ER Additional information</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,6 +661,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,13 +1066,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBB40E6-F06B-AE48-B869-B32AACDBDD09}">
-  <dimension ref="A1:AI30"/>
+  <dimension ref="A1:AH32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="24" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="41" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1107,11 +1116,11 @@
   <sheetData>
     <row r="1" spans="1:34" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
-        <v>70</v>
+      <c r="C1" s="48" t="s">
+        <v>111</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="4"/>
@@ -1147,7 +1156,7 @@
     </row>
     <row r="2" spans="1:34" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1241,7 +1250,7 @@
     </row>
     <row r="3" spans="1:34" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1313,14 +1322,14 @@
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="18"/>
@@ -1331,17 +1340,17 @@
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
       <c r="O5" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
       <c r="R5" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="S5" s="18"/>
       <c r="T5" s="18"/>
       <c r="U5" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="V5" s="18"/>
       <c r="W5" s="18"/>
@@ -1352,7 +1361,7 @@
       <c r="AB5" s="18"/>
       <c r="AC5" s="18"/>
       <c r="AD5" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AE5" s="18"/>
       <c r="AF5" s="18"/>
@@ -1361,7 +1370,7 @@
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1377,7 +1386,7 @@
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P6" s="18"/>
       <c r="Q6" s="18"/>
@@ -1394,7 +1403,7 @@
       <c r="AB6" s="18"/>
       <c r="AC6" s="18"/>
       <c r="AD6" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AE6" s="18"/>
       <c r="AF6" s="18"/>
@@ -1403,7 +1412,7 @@
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1419,7 +1428,7 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P7" s="18"/>
       <c r="Q7" s="18"/>
@@ -1436,7 +1445,7 @@
       <c r="AB7" s="18"/>
       <c r="AC7" s="18"/>
       <c r="AD7" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="AE7" s="18"/>
       <c r="AF7" s="18"/>
@@ -1445,7 +1454,7 @@
     </row>
     <row r="8" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1461,7 +1470,7 @@
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
@@ -1485,7 +1494,7 @@
     </row>
     <row r="9" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1523,7 +1532,7 @@
     </row>
     <row r="10" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1597,58 +1606,58 @@
     </row>
     <row r="12" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="L12" s="19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
       <c r="O12" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
       <c r="R12" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
       <c r="U12" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
       <c r="X12" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Y12" s="19"/>
       <c r="Z12" s="19"/>
       <c r="AA12" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
       <c r="AD12" s="19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="AE12" s="19"/>
       <c r="AF12" s="19"/>
@@ -1657,58 +1666,58 @@
     </row>
     <row r="13" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
       <c r="L13" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
       <c r="O13" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="S13" s="20"/>
       <c r="T13" s="20"/>
       <c r="U13" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="V13" s="20"/>
       <c r="W13" s="20"/>
       <c r="X13" s="20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Y13" s="20"/>
       <c r="Z13" s="20"/>
       <c r="AA13" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="AB13" s="20"/>
       <c r="AC13" s="20"/>
       <c r="AD13" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AE13" s="20"/>
       <c r="AF13" s="20"/>
@@ -1717,13 +1726,13 @@
     </row>
     <row r="14" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>76</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -1759,13 +1768,13 @@
     </row>
     <row r="15" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -1801,58 +1810,58 @@
     </row>
     <row r="16" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+        <v>75</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="40" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G16" s="41"/>
       <c r="H16" s="41"/>
       <c r="I16" s="41" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J16" s="41"/>
       <c r="K16" s="41"/>
       <c r="L16" s="40" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M16" s="41"/>
       <c r="N16" s="41"/>
       <c r="O16" s="41" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="P16" s="41"/>
       <c r="Q16" s="41"/>
       <c r="R16" s="41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="S16" s="41"/>
       <c r="T16" s="41"/>
       <c r="U16" s="40" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="V16" s="41"/>
       <c r="W16" s="41"/>
       <c r="X16" s="42" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="Y16" s="41"/>
       <c r="Z16" s="41"/>
       <c r="AA16" s="42" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="AB16" s="41"/>
       <c r="AC16" s="41"/>
       <c r="AD16" s="42" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="AE16" s="21"/>
       <c r="AF16" s="21"/>
@@ -1861,10 +1870,10 @@
     </row>
     <row r="17" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="22"/>
@@ -1901,19 +1910,17 @@
     </row>
     <row r="18" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="15" t="s">
-        <v>37</v>
-      </c>
+      <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
@@ -1945,19 +1952,17 @@
     </row>
     <row r="19" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="21" t="s">
-        <v>38</v>
-      </c>
+      <c r="F19" s="21"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -1988,16 +1993,18 @@
       <c r="AH19" s="15"/>
     </row>
     <row r="20" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="27"/>
+      <c r="A20" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -2027,490 +2034,569 @@
       <c r="AG20" s="15"/>
       <c r="AH20" s="15"/>
     </row>
-    <row r="21" spans="1:34" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
+    <row r="21" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="15"/>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="15"/>
+      <c r="AF21" s="15"/>
+      <c r="AG21" s="15"/>
+      <c r="AH21" s="15"/>
+    </row>
+    <row r="22" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="46"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="46"/>
-      <c r="Q21" s="46"/>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46"/>
-      <c r="T21" s="46"/>
-      <c r="U21" s="46"/>
-      <c r="V21" s="46"/>
-      <c r="W21" s="46"/>
-      <c r="X21" s="46"/>
-      <c r="Y21" s="46"/>
-      <c r="Z21" s="46"/>
-      <c r="AA21" s="46"/>
-      <c r="AB21" s="46"/>
-      <c r="AC21" s="46"/>
-      <c r="AD21" s="46"/>
-      <c r="AE21" s="46"/>
-      <c r="AF21" s="46"/>
-      <c r="AG21" s="46"/>
-      <c r="AH21" s="46"/>
-    </row>
-    <row r="22" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="23"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="23"/>
-      <c r="Z22" s="23"/>
-      <c r="AA22" s="23"/>
-      <c r="AB22" s="23"/>
-      <c r="AC22" s="23"/>
-      <c r="AD22" s="23"/>
-      <c r="AE22" s="23"/>
-      <c r="AF22" s="23"/>
-      <c r="AG22" s="23"/>
-      <c r="AH22" s="23"/>
-    </row>
-    <row r="23" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="35"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-      <c r="W23" s="23"/>
-      <c r="X23" s="23"/>
-      <c r="Y23" s="23"/>
-      <c r="Z23" s="23"/>
-      <c r="AA23" s="23"/>
-      <c r="AB23" s="23"/>
-      <c r="AC23" s="23"/>
-      <c r="AD23" s="23"/>
-      <c r="AE23" s="23"/>
-      <c r="AF23" s="23"/>
-      <c r="AG23" s="23"/>
-      <c r="AH23" s="23"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="15"/>
+      <c r="AH22" s="15"/>
+    </row>
+    <row r="23" spans="1:34" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="46"/>
+      <c r="Z23" s="46"/>
+      <c r="AA23" s="46"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="46"/>
+      <c r="AD23" s="46"/>
+      <c r="AE23" s="46"/>
+      <c r="AF23" s="46"/>
+      <c r="AG23" s="46"/>
+      <c r="AH23" s="46"/>
     </row>
     <row r="24" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" t="s">
-        <v>96</v>
-      </c>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" t="s">
-        <v>96</v>
-      </c>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" t="s">
-        <v>96</v>
-      </c>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" t="s">
-        <v>96</v>
-      </c>
-      <c r="X24" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG24" s="15"/>
-      <c r="AH24" s="15"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="23"/>
+      <c r="AB24" s="23"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="23"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="23"/>
+      <c r="AH24" s="23"/>
     </row>
     <row r="25" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" t="s">
-        <v>97</v>
-      </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" t="s">
-        <v>97</v>
-      </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" t="s">
-        <v>97</v>
-      </c>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" t="s">
-        <v>97</v>
-      </c>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" t="s">
-        <v>97</v>
-      </c>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" t="s">
-        <v>97</v>
-      </c>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
-      <c r="AA25"/>
-      <c r="AB25" s="15"/>
-      <c r="AC25" s="15"/>
-      <c r="AD25" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE25" s="15"/>
-      <c r="AF25" s="15"/>
-      <c r="AG25" s="15"/>
-      <c r="AH25" s="15"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="23"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
+      <c r="AA25" s="23"/>
+      <c r="AB25" s="23"/>
+      <c r="AC25" s="23"/>
+      <c r="AD25" s="23"/>
+      <c r="AE25" s="23"/>
+      <c r="AF25" s="23"/>
+      <c r="AG25" s="23"/>
+      <c r="AH25" s="23"/>
     </row>
     <row r="26" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>91</v>
+        <v>65</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>83</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
       <c r="L26" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
       <c r="O26" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
       <c r="R26" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
       <c r="U26" t="s">
-        <v>66</v>
-      </c>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
+        <v>92</v>
+      </c>
       <c r="X26" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y26" s="15"/>
-      <c r="Z26" s="15"/>
+        <v>96</v>
+      </c>
       <c r="AA26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB26" s="15"/>
-      <c r="AC26" s="15"/>
+        <v>101</v>
+      </c>
       <c r="AD26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE26" s="15"/>
-      <c r="AF26" s="15"/>
+        <v>99</v>
+      </c>
       <c r="AG26" s="15"/>
       <c r="AH26" s="15"/>
     </row>
-    <row r="27" spans="1:34" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C27" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
       <c r="I27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
       <c r="L27" t="s">
-        <v>98</v>
-      </c>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
       <c r="O27" t="s">
-        <v>98</v>
-      </c>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
       <c r="R27" t="s">
-        <v>98</v>
-      </c>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
       <c r="U27" t="s">
-        <v>98</v>
-      </c>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
+        <v>93</v>
+      </c>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
       <c r="X27" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y27" s="16"/>
-      <c r="Z27" s="16"/>
-      <c r="AA27" t="s">
-        <v>98</v>
-      </c>
-      <c r="AB27" s="16"/>
-      <c r="AC27" s="16"/>
+        <v>97</v>
+      </c>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="15"/>
       <c r="AD27" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE27" s="16"/>
-      <c r="AF27" s="16"/>
-      <c r="AG27" s="16"/>
-      <c r="AH27" s="16"/>
-    </row>
-    <row r="28" spans="1:34" s="26" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="AE27" s="15"/>
+      <c r="AF27" s="15"/>
+      <c r="AG27" s="15"/>
+      <c r="AH27" s="15"/>
+    </row>
+    <row r="28" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
+        <v>65</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
       <c r="F28" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
       <c r="I28" t="s">
-        <v>99</v>
-      </c>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
       <c r="L28" t="s">
-        <v>99</v>
-      </c>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
       <c r="O28" t="s">
-        <v>99</v>
-      </c>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
       <c r="R28" t="s">
-        <v>99</v>
-      </c>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
       <c r="U28" t="s">
-        <v>99</v>
-      </c>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
       <c r="X28" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y28" s="16"/>
-      <c r="Z28" s="16"/>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="27"/>
-      <c r="AC28" s="27"/>
-      <c r="AD28" s="27"/>
-      <c r="AE28" s="16"/>
-      <c r="AF28" s="16"/>
-      <c r="AG28" s="16"/>
-      <c r="AH28" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
+      <c r="AD28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE28" s="15"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15"/>
     </row>
     <row r="29" spans="1:34" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" t="s">
+        <v>94</v>
+      </c>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" t="s">
+        <v>94</v>
+      </c>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" t="s">
+        <v>94</v>
+      </c>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" t="s">
+        <v>94</v>
+      </c>
+      <c r="S29" s="16"/>
+      <c r="T29" s="16"/>
+      <c r="U29" t="s">
+        <v>94</v>
+      </c>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y29" s="16"/>
+      <c r="Z29" s="16"/>
+      <c r="AA29" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB29" s="16"/>
+      <c r="AC29" s="16"/>
+      <c r="AD29" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE29" s="16"/>
+      <c r="AF29" s="16"/>
+      <c r="AG29" s="16"/>
+      <c r="AH29" s="16"/>
+    </row>
+    <row r="30" spans="1:34" s="26" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
-      <c r="Z29" s="27"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="27"/>
-      <c r="AC29" s="27"/>
-      <c r="AD29" s="27"/>
-      <c r="AE29" s="27"/>
-      <c r="AF29" s="27"/>
-      <c r="AG29" s="27"/>
-      <c r="AH29" s="27"/>
-    </row>
-    <row r="30" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17"/>
-      <c r="Y30" s="17"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="17"/>
-      <c r="AB30" s="17"/>
-      <c r="AC30" s="17"/>
-      <c r="AD30" s="17"/>
-      <c r="AE30" s="17"/>
-      <c r="AF30" s="17"/>
-      <c r="AG30" s="17"/>
-      <c r="AH30" s="17"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" t="s">
+        <v>95</v>
+      </c>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" t="s">
+        <v>95</v>
+      </c>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" t="s">
+        <v>95</v>
+      </c>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" t="s">
+        <v>95</v>
+      </c>
+      <c r="S30" s="16"/>
+      <c r="T30" s="16"/>
+      <c r="U30" t="s">
+        <v>95</v>
+      </c>
+      <c r="V30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y30" s="16"/>
+      <c r="Z30" s="16"/>
+      <c r="AA30" s="27"/>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27"/>
+      <c r="AD30" s="27"/>
+      <c r="AE30" s="16"/>
+      <c r="AF30" s="16"/>
+      <c r="AG30" s="16"/>
+      <c r="AH30" s="16"/>
+    </row>
+    <row r="31" spans="1:34" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="P31" s="27"/>
+      <c r="Q31" s="27"/>
+      <c r="R31" s="27"/>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27"/>
+      <c r="U31" s="27"/>
+      <c r="V31" s="27"/>
+      <c r="W31" s="27"/>
+      <c r="X31" s="27"/>
+      <c r="Y31" s="27"/>
+      <c r="Z31" s="27"/>
+      <c r="AA31" s="27"/>
+      <c r="AB31" s="27"/>
+      <c r="AC31" s="27"/>
+      <c r="AD31" s="27"/>
+      <c r="AE31" s="27"/>
+      <c r="AF31" s="27"/>
+      <c r="AG31" s="27"/>
+      <c r="AH31" s="27"/>
+    </row>
+    <row r="32" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17"/>
+      <c r="AD32" s="17"/>
+      <c r="AE32" s="17"/>
+      <c r="AF32" s="17"/>
+      <c r="AG32" s="17"/>
+      <c r="AH32" s="17"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1" xr:uid="{5373345D-75E2-1F4C-8BAB-137B6CC77310}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update RNASeq comp for Swobup testing purposes
</commit_message>
<xml_diff>
--- a/templates/4COM01_RNASeq/4COM01_RNASeq.xlsx
+++ b/templates/4COM01_RNASeq/4COM01_RNASeq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\4COM01_RNASeq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658C104B-D049-43BA-8F76-9B53F4C04FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23938B18-AC58-4602-A7EA-428B677B7F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM01_RNASeq" sheetId="1" r:id="rId1"/>
@@ -255,14 +255,14 @@
     <t>Oliver</t>
   </si>
   <si>
-    <t>1.1.4</t>
+    <t>1.1.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,12 +277,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -783,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -907,7 +901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11AFC42-7216-4420-8824-56B92332BA6B}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Revert "Update RNASeq comp for Swobup testing purposes"
This reverts commit 30b5517b434b56b21992be5595ee824044f760ef.
</commit_message>
<xml_diff>
--- a/templates/4COM01_RNASeq/4COM01_RNASeq.xlsx
+++ b/templates/4COM01_RNASeq/4COM01_RNASeq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\4COM01_RNASeq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23938B18-AC58-4602-A7EA-428B677B7F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658C104B-D049-43BA-8F76-9B53F4C04FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM01_RNASeq" sheetId="1" r:id="rId1"/>
@@ -255,14 +255,14 @@
     <t>Oliver</t>
   </si>
   <si>
-    <t>1.1.5</t>
+    <t>1.1.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +277,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -777,7 +783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -901,9 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11AFC42-7216-4420-8824-56B92332BA6B}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>